<commit_message>
Changed line graphs for 1s and 2s IPs to bar
</commit_message>
<xml_diff>
--- a/embedded_cl_in_1st_layer_of_ice_single_water_to_cl_saop.xlsx
+++ b/embedded_cl_in_1st_layer_of_ice_single_water_to_cl_saop.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/github_thesis_graph/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/Thesis_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2617A258-4665-0F44-AB1B-5F3D97F2A494}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FAB5A6-9294-EB4D-81CA-78B6F94C0101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1180" windowWidth="21640" windowHeight="14420" xr2:uid="{41A0B090-B6CC-EE4B-87B1-C158C411CEA8}"/>
+    <workbookView xWindow="0" yWindow="1020" windowWidth="21640" windowHeight="14420" xr2:uid="{41A0B090-B6CC-EE4B-87B1-C158C411CEA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Embedded_one_water_1s_cl_saop</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Embedded_one_water_p12_cl_saop</t>
+  </si>
+  <si>
+    <t>Embedded_one_water_p32_cl_saop</t>
   </si>
 </sst>
 </file>
@@ -388,453 +391,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894879FA-00C2-5D46-B04A-A85BFC6EEBFA}">
-  <dimension ref="B3:R28"/>
+  <dimension ref="B4:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:R28"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>2</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>2759.8826410000001</v>
-      </c>
-      <c r="F4">
-        <v>249.3458152</v>
-      </c>
-      <c r="J4">
-        <v>186.78734750000001</v>
-      </c>
-      <c r="N4">
-        <v>189.48500970000001</v>
-      </c>
-      <c r="R4">
-        <v>187.81862889999999</v>
+      <c r="R4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>2759.479711</v>
+        <v>2759.8826410000001</v>
       </c>
       <c r="F5">
-        <v>248.940877</v>
+        <v>249.3458152</v>
       </c>
       <c r="J5">
-        <v>186.87159589999999</v>
+        <v>186.78734750000001</v>
       </c>
       <c r="N5">
-        <v>189.08024900000001</v>
+        <v>189.48500970000001</v>
       </c>
       <c r="R5">
-        <v>187.413872</v>
+        <v>187.81862889999999</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>2758.8669140000002</v>
+        <v>2759.479711</v>
       </c>
       <c r="F6">
-        <v>248.3344568</v>
+        <v>248.940877</v>
       </c>
       <c r="J6">
-        <v>186.9558442</v>
+        <v>186.87159589999999</v>
       </c>
       <c r="N6">
-        <v>188.473872</v>
+        <v>189.08024900000001</v>
       </c>
       <c r="R6">
-        <v>186.8071477</v>
+        <v>187.413872</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>2759.288086</v>
+        <v>2758.8669140000002</v>
       </c>
       <c r="F7">
-        <v>248.7530677</v>
+        <v>248.3344568</v>
       </c>
       <c r="J7">
-        <v>187.04009249999999</v>
+        <v>186.9558442</v>
       </c>
       <c r="N7">
-        <v>188.89271439999999</v>
+        <v>188.473872</v>
       </c>
       <c r="R7">
-        <v>187.22631949999999</v>
+        <v>186.8071477</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>2758.7700150000001</v>
+        <v>2759.288086</v>
       </c>
       <c r="F8">
-        <v>248.23219649999999</v>
+        <v>248.7530677</v>
       </c>
       <c r="J8">
-        <v>187.12434089999999</v>
+        <v>187.04009249999999</v>
       </c>
       <c r="N8">
-        <v>188.3726384</v>
+        <v>188.89271439999999</v>
       </c>
       <c r="R8">
-        <v>186.70627429999999</v>
+        <v>187.22631949999999</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>2759.6221169999999</v>
+        <v>2758.7700150000001</v>
       </c>
       <c r="F9">
-        <v>249.08340419999999</v>
+        <v>248.23219649999999</v>
       </c>
       <c r="J9">
-        <v>187.20858920000001</v>
+        <v>187.12434089999999</v>
       </c>
       <c r="N9">
-        <v>189.22305449999999</v>
+        <v>188.3726384</v>
       </c>
       <c r="R9">
-        <v>187.55666729999999</v>
+        <v>186.70627429999999</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>2759.6799019999999</v>
+        <v>2759.6221169999999</v>
       </c>
       <c r="F10">
-        <v>249.15170739999999</v>
+        <v>249.08340419999999</v>
       </c>
       <c r="J10">
-        <v>187.29283749999999</v>
+        <v>187.20858920000001</v>
       </c>
       <c r="N10">
-        <v>189.29120030000001</v>
+        <v>189.22305449999999</v>
       </c>
       <c r="R10">
-        <v>187.6248544</v>
+        <v>187.55666729999999</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>2758.6292450000001</v>
+        <v>2759.6799019999999</v>
       </c>
       <c r="F11">
-        <v>248.09402109999999</v>
+        <v>249.15170739999999</v>
       </c>
       <c r="J11">
-        <v>187.3770858</v>
+        <v>187.29283749999999</v>
       </c>
       <c r="N11">
-        <v>188.23427599999999</v>
+        <v>189.29120030000001</v>
       </c>
       <c r="R11">
-        <v>186.56791659999999</v>
+        <v>187.6248544</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>2759.3601629999998</v>
+        <v>2758.6292450000001</v>
       </c>
       <c r="F12">
-        <v>248.81885750000001</v>
+        <v>248.09402109999999</v>
       </c>
       <c r="J12">
-        <v>187.46133420000001</v>
+        <v>187.3770858</v>
       </c>
       <c r="N12">
-        <v>188.95876720000001</v>
+        <v>188.23427599999999</v>
       </c>
       <c r="R12">
-        <v>187.29238620000001</v>
+        <v>186.56791659999999</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13">
-        <v>2759.3202150000002</v>
+        <v>2759.3601629999998</v>
       </c>
       <c r="F13">
-        <v>248.79077029999999</v>
+        <v>248.81885750000001</v>
       </c>
       <c r="J13">
-        <v>187.54558249999999</v>
+        <v>187.46133420000001</v>
       </c>
       <c r="N13">
-        <v>188.92974659999999</v>
+        <v>188.95876720000001</v>
       </c>
       <c r="R13">
-        <v>187.2633874</v>
+        <v>187.29238620000001</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>2759.5064139999999</v>
+        <v>2759.3202150000002</v>
       </c>
       <c r="F14">
-        <v>248.97517999999999</v>
+        <v>248.79077029999999</v>
       </c>
       <c r="J14">
-        <v>187.62983080000001</v>
+        <v>187.54558249999999</v>
       </c>
       <c r="N14">
-        <v>189.1145247</v>
+        <v>188.92974659999999</v>
       </c>
       <c r="R14">
-        <v>187.44816940000001</v>
+        <v>187.2633874</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15">
-        <v>2755.5455149999998</v>
+        <v>2759.5064139999999</v>
       </c>
       <c r="F15">
-        <v>245.09536750000001</v>
+        <v>248.97517999999999</v>
       </c>
       <c r="J15">
-        <v>187.71407919999999</v>
+        <v>187.62983080000001</v>
       </c>
       <c r="N15">
-        <v>185.21672430000001</v>
+        <v>189.1145247</v>
       </c>
       <c r="R15">
-        <v>183.5485827</v>
+        <v>187.44816940000001</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>2758.4798270000001</v>
+        <v>2755.5455149999998</v>
       </c>
       <c r="F16">
-        <v>247.94295389999999</v>
+        <v>245.09536750000001</v>
       </c>
       <c r="J16">
-        <v>187.7983275</v>
+        <v>187.71407919999999</v>
       </c>
       <c r="N16">
-        <v>188.08357810000001</v>
+        <v>185.21672430000001</v>
       </c>
       <c r="R16">
-        <v>186.4172183</v>
+        <v>183.5485827</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17">
-        <v>2758.4930530000001</v>
+        <v>2758.4798270000001</v>
       </c>
       <c r="F17">
-        <v>247.9518913</v>
+        <v>247.94295389999999</v>
       </c>
       <c r="J17">
-        <v>187.88257580000001</v>
+        <v>187.7983275</v>
       </c>
       <c r="N17">
-        <v>188.0923449</v>
+        <v>188.08357810000001</v>
       </c>
       <c r="R17">
-        <v>186.42596879999999</v>
+        <v>186.4172183</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18">
-        <v>2759.877786</v>
+        <v>2758.4930530000001</v>
       </c>
       <c r="F18">
-        <v>249.34136849999999</v>
+        <v>247.9518913</v>
       </c>
       <c r="J18">
-        <v>187.96682419999999</v>
+        <v>187.88257580000001</v>
       </c>
       <c r="N18">
-        <v>189.48069079999999</v>
+        <v>188.0923449</v>
       </c>
       <c r="R18">
-        <v>187.81430710000001</v>
+        <v>186.42596879999999</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19">
-        <v>2759.6327150000002</v>
+        <v>2759.877786</v>
       </c>
       <c r="F19">
-        <v>249.09645320000001</v>
+        <v>249.34136849999999</v>
       </c>
       <c r="J19">
-        <v>188.0510725</v>
+        <v>187.96682419999999</v>
       </c>
       <c r="N19">
-        <v>189.23624150000001</v>
+        <v>189.48069079999999</v>
       </c>
       <c r="R19">
-        <v>187.5698764</v>
+        <v>187.81430710000001</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20">
-        <v>2759.129778</v>
+        <v>2759.6327150000002</v>
       </c>
       <c r="F20">
-        <v>248.59259170000001</v>
+        <v>249.09645320000001</v>
       </c>
       <c r="J20">
-        <v>188.13532079999999</v>
+        <v>188.0510725</v>
       </c>
       <c r="N20">
-        <v>188.73267100000001</v>
+        <v>189.23624150000001</v>
       </c>
       <c r="R20">
-        <v>187.06630530000001</v>
+        <v>187.5698764</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21">
-        <v>2760.302768</v>
+        <v>2759.129778</v>
       </c>
       <c r="F21">
-        <v>249.77248599999999</v>
+        <v>248.59259170000001</v>
       </c>
       <c r="J21">
-        <v>188.2195692</v>
+        <v>188.13532079999999</v>
       </c>
       <c r="N21">
-        <v>189.91166150000001</v>
+        <v>188.73267100000001</v>
       </c>
       <c r="R21">
-        <v>188.24530440000001</v>
+        <v>187.06630530000001</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>2757.6500329999999</v>
+        <v>2760.302768</v>
       </c>
       <c r="F22">
-        <v>247.10440439999999</v>
+        <v>249.77248599999999</v>
       </c>
       <c r="J22">
-        <v>188.30381750000001</v>
+        <v>188.2195692</v>
       </c>
       <c r="N22">
-        <v>187.24508</v>
+        <v>189.91166150000001</v>
       </c>
       <c r="R22">
-        <v>185.57869009999999</v>
+        <v>188.24530440000001</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23">
-        <v>2757.6346309999999</v>
+        <v>2757.6500329999999</v>
       </c>
       <c r="F23">
-        <v>247.07809219999999</v>
+        <v>247.10440439999999</v>
       </c>
       <c r="J23">
-        <v>188.38806579999999</v>
+        <v>188.30381750000001</v>
       </c>
       <c r="N23">
-        <v>187.2186298</v>
+        <v>187.24508</v>
       </c>
       <c r="R23">
-        <v>185.55219500000001</v>
+        <v>185.57869009999999</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24">
-        <v>2758.4846459999999</v>
+        <v>2757.6346309999999</v>
       </c>
       <c r="F24">
-        <v>247.9298383</v>
+        <v>247.07809219999999</v>
       </c>
       <c r="J24">
-        <v>188.4723142</v>
+        <v>188.38806579999999</v>
       </c>
       <c r="N24">
-        <v>188.07008669999999</v>
+        <v>187.2186298</v>
       </c>
       <c r="R24">
-        <v>186.4036543</v>
+        <v>185.55219500000001</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25">
-        <v>2758.3216000000002</v>
+        <v>2758.4846459999999</v>
       </c>
       <c r="F25">
-        <v>247.77225720000001</v>
+        <v>247.9298383</v>
       </c>
       <c r="J25">
-        <v>188.55656250000001</v>
+        <v>188.4723142</v>
       </c>
       <c r="N25">
-        <v>187.9122079</v>
+        <v>188.07008669999999</v>
       </c>
       <c r="R25">
-        <v>186.24579220000001</v>
+        <v>186.4036543</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>2759.9500889999999</v>
+        <v>2758.3216000000002</v>
       </c>
       <c r="F26">
-        <v>249.41048119999999</v>
+        <v>247.77225720000001</v>
       </c>
       <c r="J26">
-        <v>188.6408108</v>
+        <v>188.55656250000001</v>
       </c>
       <c r="N26">
-        <v>189.55056049999999</v>
+        <v>187.9122079</v>
       </c>
       <c r="R26">
-        <v>187.88418630000001</v>
+        <v>186.24579220000001</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27">
-        <v>2759.8807630000001</v>
+        <v>2759.9500889999999</v>
       </c>
       <c r="F27">
-        <v>249.34556520000001</v>
+        <v>249.41048119999999</v>
       </c>
       <c r="J27">
-        <v>188.7250592</v>
+        <v>188.6408108</v>
       </c>
       <c r="N27">
-        <v>189.48468700000001</v>
+        <v>189.55056049999999</v>
       </c>
       <c r="R27">
-        <v>187.81831320000001</v>
+        <v>187.88418630000001</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28">
+        <v>2759.8807630000001</v>
+      </c>
+      <c r="F28">
+        <v>249.34556520000001</v>
+      </c>
+      <c r="J28">
+        <v>188.7250592</v>
+      </c>
+      <c r="N28">
+        <v>189.48468700000001</v>
+      </c>
+      <c r="R28">
+        <v>187.81831320000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B29">
         <v>2759.889036</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>249.3583442</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>188.80930749999999</v>
       </c>
-      <c r="N28">
+      <c r="N29">
         <v>189.49774489999999</v>
       </c>
-      <c r="R28">
+      <c r="R29">
         <v>187.83139600000001</v>
       </c>
     </row>

</xml_diff>